<commit_message>
Seprate Folders For each Employee
</commit_message>
<xml_diff>
--- a/Global_Variables.xlsx
+++ b/Global_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\PAYSTUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1229CD72-1933-49A0-94DD-39ACD49E2D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C00C96-EE77-4BC8-90B8-BB03CC3D2102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Employee_Name</t>
   </si>
@@ -47,6 +47,27 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>kamil</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc </t>
+  </si>
+  <si>
+    <t>doc_options</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>paystub_options</t>
+  </si>
+  <si>
+    <t>{"Rate" : "", "Numbe of Paystubs":"", "Period" : "",  }</t>
   </si>
 </sst>
 </file>
@@ -887,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,9 +921,10 @@
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -918,8 +940,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -934,9 +962,50 @@
       </c>
       <c r="E2">
         <v>123456789</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>111222333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>222555888</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Paystub Creation Error Solved
</commit_message>
<xml_diff>
--- a/Global_Variables.xlsx
+++ b/Global_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\PAYSTUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C00C96-EE77-4BC8-90B8-BB03CC3D2102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F23D9C-C7C9-4595-86CA-71360369DB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,10 +64,10 @@
     <t>1,2,3</t>
   </si>
   <si>
-    <t>paystub_options</t>
-  </si>
-  <si>
-    <t>{"Rate" : "", "Numbe of Paystubs":"", "Period" : "",  }</t>
+    <t>paystub_A_options</t>
+  </si>
+  <si>
+    <t>{"Rate" : 20 , "4_Digit_Account_Number" : 8698, "Numbe of Paystubs" : 5, "Period" : "Apr 01 2022"}</t>
   </si>
 </sst>
 </file>
@@ -911,7 +911,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Excel Automation with All Paystubs
</commit_message>
<xml_diff>
--- a/Global_Variables.xlsx
+++ b/Global_Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\PAYSTUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F23D9C-C7C9-4595-86CA-71360369DB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B8DD1C-D607-41C4-99C4-F9E4AB08C01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_Variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Employee_Name</t>
   </si>
@@ -61,13 +61,28 @@
     <t>doc_options</t>
   </si>
   <si>
-    <t>1,2,3</t>
-  </si>
-  <si>
     <t>paystub_A_options</t>
   </si>
   <si>
     <t>{"Rate" : 20 , "4_Digit_Account_Number" : 8698, "Numbe of Paystubs" : 5, "Period" : "Apr 01 2022"}</t>
+  </si>
+  <si>
+    <t>{"Rate" : 30 , "4_Digit_Account_Number" : 8698, "Numbe of Paystubs" : 3, "Period" : "Apr 01 2022"}</t>
+  </si>
+  <si>
+    <t>{"Rate" : 25 , "4_Digit_Account_Number" : 8698, "Numbe of Paystubs" : 5, "Period" : "Apr 01 2022"}</t>
+  </si>
+  <si>
+    <t>paystub_B_options</t>
+  </si>
+  <si>
+    <t>{"Rate" : 20 , "occupation" : "Student", "Numbe of Paystubs" : 5, "Period" : "Apr 01 2022"}</t>
+  </si>
+  <si>
+    <t>paystub_C_options</t>
+  </si>
+  <si>
+    <t>{"Rate" : 20 , "Numbe of Paystubs" : 5, "Period" : "Apr 01 2022"}</t>
   </si>
 </sst>
 </file>
@@ -908,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,7 +939,7 @@
     <col min="6" max="6" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -944,10 +959,16 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -963,14 +984,20 @@
       <c r="E2">
         <v>123456789</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -986,8 +1013,20 @@
       <c r="E3">
         <v>111222333</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1002,6 +1041,18 @@
       </c>
       <c r="E4">
         <v>222555888</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>